<commit_message>
add to under-represented count vols and format
</commit_message>
<xml_diff>
--- a/data/turning_counts/int100.xlsx
+++ b/data/turning_counts/int100.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydenatchley/Documents/662_dogbones_2023/data/turning_counts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85C29829-0A96-EC4F-BC3D-F58686A6E8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DBE3DD-AD93-0142-849B-A3241F8A6355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="17100" windowHeight="10120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="17100" windowHeight="10120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Info" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
     <sheet name="Bank4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="80000"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -259,8 +248,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="8.25"/>
       <name val="Arial"/>
@@ -268,17 +257,20 @@
     <font>
       <sz val="8.25"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8.25"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8.25"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -290,6 +282,13 @@
       <b/>
       <sz val="8.25"/>
       <name val="Microsoft Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="8.25"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -320,7 +319,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -378,6 +377,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -728,7 +731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0"/>
@@ -820,12 +823,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -953,8 +956,8 @@
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="9">
-        <v>0</v>
+      <c r="C3" s="15">
+        <v>1</v>
       </c>
       <c r="D3" s="9">
         <v>18</v>
@@ -1402,7 +1405,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="0" orientation="portrait" blackAndWhite="1" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1411,7 +1413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2001,7 +2003,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2583,7 +2585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>